<commit_message>
wrote u genre names
</commit_message>
<xml_diff>
--- a/power_plant_power_calculated_Q_values.xlsx
+++ b/power_plant_power_calculated_Q_values.xlsx
@@ -14,7 +14,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="20">
+  <si>
+    <t>U (PE-D)</t>
+  </si>
+  <si>
+    <t>U (HG-S)</t>
+  </si>
+  <si>
+    <t>U (HG-D)</t>
+  </si>
+  <si>
+    <t>U (PC-S)</t>
+  </si>
+  <si>
+    <t>U (PC-D)</t>
+  </si>
+  <si>
+    <t>U (PVC-S)</t>
+  </si>
+  <si>
+    <t>U (PVC-D)</t>
+  </si>
   <si>
     <t>Ocak</t>
   </si>
@@ -384,357 +405,383 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>-3570571.112500001</v>
-      </c>
-      <c r="C1">
-        <v>-3317545.40625</v>
-      </c>
-      <c r="D1">
-        <v>-3841523.775</v>
-      </c>
-      <c r="E1">
-        <v>-3625946.85625</v>
-      </c>
-      <c r="F1">
-        <v>-3211590.287500001</v>
-      </c>
-      <c r="G1">
-        <v>-2969767.90625</v>
-      </c>
-      <c r="H1">
-        <v>-3842415.66875</v>
-      </c>
-      <c r="I1">
-        <v>-3601201.325</v>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>-3623530.987500001</v>
+        <v>-3570571.112500001</v>
       </c>
       <c r="C2">
-        <v>-3345309.700000001</v>
+        <v>-3317545.40625</v>
       </c>
       <c r="D2">
-        <v>-3887139.9625</v>
+        <v>-3841523.775</v>
       </c>
       <c r="E2">
-        <v>-3642621.9375</v>
+        <v>-3625946.85625</v>
       </c>
       <c r="F2">
-        <v>-3261442.3375</v>
+        <v>-3211590.287500001</v>
       </c>
       <c r="G2">
-        <v>-2997532.2</v>
+        <v>-2969767.90625</v>
       </c>
       <c r="H2">
-        <v>-3894376.600000001</v>
+        <v>-3842415.66875</v>
       </c>
       <c r="I2">
-        <v>-3624858.850000001</v>
+        <v>-3601201.325</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>-3965486.875</v>
+        <v>-3623530.987500001</v>
       </c>
       <c r="C3">
-        <v>-3518840.5</v>
+        <v>-3345309.700000001</v>
       </c>
       <c r="D3">
-        <v>-4181066.875</v>
+        <v>-3887139.9625</v>
       </c>
       <c r="E3">
-        <v>-3745449.0625</v>
+        <v>-3642621.9375</v>
       </c>
       <c r="F3">
-        <v>-3582975.375</v>
+        <v>-3261442.3375</v>
       </c>
       <c r="G3">
-        <v>-3171063</v>
+        <v>-2997532.2</v>
       </c>
       <c r="H3">
-        <v>-4231670.75</v>
+        <v>-3894376.600000001</v>
       </c>
       <c r="I3">
-        <v>-3773305.0625</v>
+        <v>-3624858.850000001</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>-4369504.125</v>
+        <v>-3965486.875</v>
       </c>
       <c r="C4">
-        <v>-3723956.95</v>
+        <v>-3518840.5</v>
       </c>
       <c r="D4">
-        <v>-4527078.625</v>
+        <v>-4181066.875</v>
       </c>
       <c r="E4">
-        <v>-3860786.3125</v>
+        <v>-3745449.0625</v>
       </c>
       <c r="F4">
-        <v>-3962130.025</v>
+        <v>-3582975.375</v>
       </c>
       <c r="G4">
-        <v>-3376179.45</v>
+        <v>-3171063</v>
       </c>
       <c r="H4">
-        <v>-4625920.55</v>
+        <v>-4231670.75</v>
       </c>
       <c r="I4">
-        <v>-3943791.4625</v>
+        <v>-3773305.0625</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>-4369504.125</v>
+      </c>
+      <c r="C5">
+        <v>-3723956.95</v>
+      </c>
+      <c r="D5">
+        <v>-4527078.625</v>
+      </c>
+      <c r="E5">
+        <v>-3860786.3125</v>
+      </c>
+      <c r="F5">
+        <v>-3962130.025</v>
+      </c>
+      <c r="G5">
+        <v>-3376179.45</v>
+      </c>
+      <c r="H5">
+        <v>-4625920.55</v>
+      </c>
+      <c r="I5">
+        <v>-3943791.4625</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I10" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
         <v>-3824651.662500001</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>-3445489.487500001</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>-4060054.3</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>-3702701.05</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>-3450575.6875</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>-3097711.9875</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <v>-4094149.49375</v>
       </c>
-      <c r="I12">
+      <c r="I13">
         <v>-3711703.53125</v>
       </c>
     </row>

</xml_diff>